<commit_message>
Initial ImportedEvent, KilledEvent, changed RatedEvent, some other changes
</commit_message>
<xml_diff>
--- a/prospero-database/sample/sample-data.xlsx
+++ b/prospero-database/sample/sample-data.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ws-sma-bd01\JackCoady\MainProjects\AllSpark\Billing\prospero-database\sample\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ws-sma-bd01\JackCoady\MainProjects\AllSpark\Billing\prospero-database\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18195" windowHeight="9000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18195" windowHeight="9000"/>
   </bookViews>
   <sheets>
-    <sheet name="Customer" sheetId="1" r:id="rId1"/>
-    <sheet name="Address" sheetId="2" r:id="rId2"/>
-    <sheet name="CustomerProductCharge" sheetId="3" r:id="rId3"/>
-    <sheet name="BillingReference" sheetId="4" r:id="rId4"/>
+    <sheet name="SOURCES" sheetId="6" r:id="rId1"/>
+    <sheet name="Customer" sheetId="1" r:id="rId2"/>
+    <sheet name="Address" sheetId="2" r:id="rId3"/>
+    <sheet name="CustomerProductCharge" sheetId="3" r:id="rId4"/>
     <sheet name="RatedEvent" sheetId="5" r:id="rId5"/>
+    <sheet name="BillingReference" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3732" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3823" uniqueCount="558">
   <si>
     <t>CustomerID</t>
   </si>
@@ -1597,6 +1598,111 @@
   </si>
   <si>
     <t>Credit for Call Charges</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Ganymede Eclipse Extract</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>CustomerProductCharge</t>
+  </si>
+  <si>
+    <t>RatedEvent (until new system does it)</t>
+  </si>
+  <si>
+    <t>Eclipse</t>
+  </si>
+  <si>
+    <t>BillingReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NumberRangeMap </t>
+  </si>
+  <si>
+    <t>BD01 (until program writes to mysql)</t>
+  </si>
+  <si>
+    <t>CustomerID,AccountNumber,Company,AddressID=CustomerID from vw_customers2</t>
+  </si>
+  <si>
+    <t>AddressID=CustomerID,Line1,Line2,Town,County,Country,Postcode from vw_customers2</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>Ganymede Eclipse, vw_customers2</t>
+  </si>
+  <si>
+    <t>Town</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>Address3</t>
+  </si>
+  <si>
+    <t>join Customers</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Tel_ID</t>
+  </si>
+  <si>
+    <t>(BT_OrderNo or CPS_OrderNo or …)</t>
+  </si>
+  <si>
+    <t>Ganymede Eclipse, BillCharges</t>
+  </si>
+  <si>
+    <t>Product_ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>join Products</t>
+  </si>
+  <si>
+    <t>Repeet</t>
+  </si>
+  <si>
+    <t>PriceCost</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>LastTo</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>(join BillingRefAttr, User_ContractDate + Len?)</t>
+  </si>
+  <si>
+    <t>(join BillingRefAttr, SP_ContractDate + Len?)</t>
+  </si>
+  <si>
+    <t>(join BillingRefAttr, Description? Needs clean - "Not Provided" etc)</t>
   </si>
 </sst>
 </file>
@@ -1640,12 +1746,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1926,10 +2033,390 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>534</v>
+      </c>
+      <c r="D3" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>536</v>
+      </c>
+      <c r="C12" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>419</v>
+      </c>
+      <c r="C15" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="D34" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="D36" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="D38" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>525</v>
+      </c>
+      <c r="C48" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>526</v>
+      </c>
+      <c r="C49" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>529</v>
+      </c>
+      <c r="C50" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>527</v>
+      </c>
+      <c r="C51" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>530</v>
+      </c>
+      <c r="C53" t="s">
+        <v>531</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DV73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="A2:D6"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4360,7 +4847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G74"/>
   <sheetViews>
@@ -6068,12 +6555,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y490"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="R1" workbookViewId="0">
+      <selection sqref="A1:X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42372,7 +42859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -42384,7 +42871,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>